<commit_message>
Prod type updated Week 3 Aug24
</commit_message>
<xml_diff>
--- a/0. Prod Inventory/Product Type_MY.xlsx
+++ b/0. Prod Inventory/Product Type_MY.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nactuarialsolutions.sharepoint.com/sites/intern/Shared Documents/General/Wilson/Web Scraping Local/Product Type/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nactuarialsolutions.sharepoint.com/sites/intern/Shared Documents/General/Product/web-scraper/0. Prod Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2852" documentId="13_ncr:1_{E59A9F57-7555-41DB-AD1E-6C065A761BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{351880D6-8B52-40DE-AA95-F43A3D298BF7}"/>
+  <xr:revisionPtr revIDLastSave="2893" documentId="13_ncr:1_{E59A9F57-7555-41DB-AD1E-6C065A761BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD6756BA-CFBE-4CDD-A94B-24851EFCDC68}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{70525E09-F0DC-4855-ADF9-7EA5A6A61783}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="4" activeTab="4" xr2:uid="{70525E09-F0DC-4855-ADF9-7EA5A6A61783}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="9" r:id="rId1"/>
@@ -95,8 +95,40 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1799" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="685">
   <si>
     <t>Insurance Company</t>
   </si>
@@ -3933,6 +3965,215 @@
 Your policy will not lapse within the first six (6) policy years or during the premium payment term, whichever is earlier, from the effective date if the Account Value is less than or equal to zero (0) on the due date of the monthly policy fee and insurance charge provided that:
 i. All premiums of the policy due have been paid on each premium due date or within the grace period of thirty (30) days from the premium due date; and
 ii. No partial withdrawal from the Protection Account is performed.</t>
+    </r>
+  </si>
+  <si>
+    <t>Banca - Alliance</t>
+  </si>
+  <si>
+    <t>14d - 70y</t>
+  </si>
+  <si>
+    <t>Minimum RM35k per year</t>
+  </si>
+  <si>
+    <t>Up to 99y.
+TPD coverage up to 70y.</t>
+  </si>
+  <si>
+    <t>Varies by payment frequency:
+Monthly: RM6.00
+Others: RM5.00</t>
+  </si>
+  <si>
+    <t>Deducted from IPA based on the % of amount withdrawn from IPA.</t>
+  </si>
+  <si>
+    <t>Deducted based on % of IPA AV.</t>
+  </si>
+  <si>
+    <t>Varies</t>
+  </si>
+  <si>
+    <t>Waived</t>
+  </si>
+  <si>
+    <t>0.75% - 1.50%</t>
+  </si>
+  <si>
+    <t>3.75% of insurance premiums</t>
+  </si>
+  <si>
+    <t>Max (200% of Insurance Premium, Total AV)</t>
+  </si>
+  <si>
+    <t>Additional of:
+i. 100% of ADB Face Amount (All causes)
+ii. 200% of ADB Face Amount (Public Conveyance)
+*ADB Face Amount = 200%*Annualised Insurance Premium*3</t>
+  </si>
+  <si>
+    <t>Total AV + 10% IPA Value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Loyalty Bonus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of 2.0% of total AV every 5y starting from policy yaer 10.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Auto Fund Rebalancing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Investment portfolio will be rebalanced every quarter to ensure that the portfolio mix you have chosen remains consistent.</t>
+    </r>
+  </si>
+  <si>
+    <t>Manulife Future Shield</t>
+  </si>
+  <si>
+    <t>19y - 55y</t>
+  </si>
+  <si>
+    <t>Up to 99y</t>
+  </si>
+  <si>
+    <t>Policy Y1-Y2: Total Premium Paid (TPP)
+&lt;70y: 105% of TPP
+&gt;=70y: BSA</t>
+  </si>
+  <si>
+    <t>Policy Y1-Y2: Total Premium Paid (TPP)
+&lt;70y: 105% of TPP
+&gt;=70y: N/A</t>
+  </si>
+  <si>
+    <t>Face Amount</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Withdrawal Benefits: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Basic Premium - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">100% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>will be allocated into the Insurance Premium Account (IPA) according to chosen funds
+Top-up Premium - 95% will be allocated into the Top-Up Premium Account (TUPA) according to chosen funds
+Total AV = IPA + TUPA</t>
+    </r>
+  </si>
+  <si>
+    <t>SIO up to RM2 million.</t>
+  </si>
+  <si>
+    <t>EliteLife Signature Treasure</t>
+  </si>
+  <si>
+    <t>Policy Y1-Y2: Face Amount
+&lt;70y: Face Amount
+&gt;=70y: N/A
+Entry Age | Face Amount
+19 - 29 | 500% of TPP
+30 - 39 | 300% of TPP
+40 - 49 | 250% of TPP
+50 - 55 | 200% of TPP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Senior Care Benefit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Policy Y1-Y2: N/A
+&lt;70y: N/A
+&gt;=70y: Face Amount</t>
     </r>
   </si>
 </sst>
@@ -4204,7 +4445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4358,7 +4599,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4856,10 +5105,147 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>27372</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>361951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2109788</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1770028</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{985E58D8-4DB1-4B9F-8C0C-9908E575E547}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10438197" y="13215939"/>
+          <a:ext cx="2082416" cy="1408077"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>319088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2130041</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1727165</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DC71321-24D1-4FD4-B1BD-437DF7E30433}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10458450" y="14992351"/>
+          <a:ext cx="2082416" cy="1408077"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>189017</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>217713</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4403201</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>3899805</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9E97769-057F-4286-9E92-C5C1748F4661}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10885592" y="14548076"/>
+          <a:ext cx="4272288" cy="3673929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4996,7 +5382,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5049,6 +5435,75 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Alistair Fang" id="{5D152006-4A03-4644-B3FC-AFEE224E7A31}" userId="S::alistair.fang@actomate.ai::78864434-0cf2-4820-8063-63d30832ffb1" providerId="AD"/>
 </personList>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5886,7 +6341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313B3ADD-1C7B-473A-99A9-A861CDD224A1}">
   <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="J2" sqref="J2"/>
     </sheetView>
@@ -6555,7 +7010,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6577,7 +7032,7 @@
       <c r="D2" s="36" t="s">
         <v>517</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="36" t="s">
         <v>617</v>
       </c>
     </row>
@@ -6986,13 +7441,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48281F2A-1CEE-4910-884C-6FE42D909869}">
-  <dimension ref="B2:E32"/>
+  <dimension ref="B2:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7002,11 +7457,12 @@
     <col min="3" max="3" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="18.21875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="31" style="1" customWidth="1"/>
+    <col min="7" max="10" width="18.21875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -7019,8 +7475,11 @@
       <c r="E2" s="9" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="56" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
@@ -7033,8 +7492,11 @@
       <c r="E3" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
@@ -7047,8 +7509,11 @@
       <c r="E4" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -7061,8 +7526,11 @@
       <c r="E5" s="9" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="9" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -7075,8 +7543,11 @@
       <c r="E6" s="9" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -7089,8 +7560,11 @@
       <c r="E7" s="9" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -7103,8 +7577,11 @@
       <c r="E8" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -7117,8 +7594,11 @@
       <c r="E9" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="F9" s="9" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>390</v>
       </c>
@@ -7131,8 +7611,11 @@
       <c r="E10" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="5" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -7145,8 +7628,11 @@
       <c r="E11" s="5" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="5" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -7159,8 +7645,11 @@
       <c r="E12" s="5" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
@@ -7173,8 +7662,11 @@
       <c r="E13" s="5" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="F13" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -7187,8 +7679,11 @@
       <c r="E14" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="5" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -7201,8 +7696,11 @@
       <c r="E15" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" ht="156" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="156" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>394</v>
       </c>
@@ -7215,8 +7713,11 @@
       <c r="E16" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="F16" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>91</v>
       </c>
@@ -7229,16 +7730,20 @@
       <c r="E17" s="28" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="55" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
         <v>225</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
-    </row>
-    <row r="19" spans="2:5" ht="263.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="37"/>
+    </row>
+    <row r="19" spans="2:6" ht="263.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>227</v>
       </c>
@@ -7251,8 +7756,11 @@
       <c r="E19" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" ht="143.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="5" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="143.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>228</v>
       </c>
@@ -7265,8 +7773,11 @@
       <c r="E20" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="149.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="5" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>229</v>
       </c>
@@ -7279,8 +7790,11 @@
       <c r="E21" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F21" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>230</v>
       </c>
@@ -7293,8 +7807,11 @@
       <c r="E22" s="39" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="39" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>232</v>
       </c>
@@ -7307,8 +7824,11 @@
       <c r="E23" s="39" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F23" s="39" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>231</v>
       </c>
@@ -7321,8 +7841,11 @@
       <c r="E24" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" ht="231" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="5" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="231" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>393</v>
       </c>
@@ -7335,16 +7858,20 @@
       <c r="E25" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="5" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
         <v>226</v>
       </c>
       <c r="C26" s="40"/>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
-    </row>
-    <row r="27" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="37"/>
+    </row>
+    <row r="27" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
@@ -7357,8 +7884,11 @@
       <c r="E27" s="5" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="F27" s="5" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
@@ -7371,8 +7901,11 @@
       <c r="E28" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="F28" s="5" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>221</v>
       </c>
@@ -7385,8 +7918,11 @@
       <c r="E29" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="5" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
@@ -7399,8 +7935,11 @@
       <c r="E30" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="F30" s="9" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
@@ -7413,8 +7952,11 @@
       <c r="E31" s="5" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" ht="372.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="5" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="372.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>14</v>
       </c>
@@ -7425,6 +7967,9 @@
         <v>64</v>
       </c>
       <c r="E32" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -7437,13 +7982,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8220FE-2D73-47FD-8C9B-E987A6F5AF90}">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:G24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7453,10 +7998,11 @@
     <col min="3" max="3" width="32" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
     <col min="5" max="6" width="30.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="64.21875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -7472,8 +8018,11 @@
       <c r="F2" s="3" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G2" s="51" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
@@ -7489,8 +8038,11 @@
       <c r="F3" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
@@ -7506,8 +8058,11 @@
       <c r="F4" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -7523,8 +8078,11 @@
       <c r="F5" s="2" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -7540,8 +8098,11 @@
       <c r="F6" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -7557,8 +8118,11 @@
       <c r="F7" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -7574,8 +8138,11 @@
       <c r="F8" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>176</v>
       </c>
@@ -7591,8 +8158,11 @@
       <c r="F9" s="2" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G9" s="2" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -7608,8 +8178,11 @@
       <c r="F10" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G10" s="2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="72" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -7625,8 +8198,11 @@
       <c r="F11" s="5" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="5" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -7642,8 +8218,11 @@
       <c r="F12" s="5" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G12" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="72" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
@@ -7659,8 +8238,11 @@
       <c r="F13" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -7676,8 +8258,11 @@
       <c r="F14" s="12" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="G14" s="12" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="144" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -7693,8 +8278,11 @@
       <c r="F15" s="5" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="G15" s="5" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="144" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -7710,8 +8298,11 @@
       <c r="F16" s="5" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G16" s="5" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="140.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>209</v>
       </c>
@@ -7727,8 +8318,11 @@
       <c r="F17" s="12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="5" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
@@ -7744,8 +8338,11 @@
       <c r="F18" s="2" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>213</v>
       </c>
@@ -7761,8 +8358,11 @@
       <c r="F19" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
@@ -7778,8 +8378,11 @@
       <c r="F20" s="2" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
@@ -7787,8 +8390,9 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" ht="255" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" ht="310.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>20</v>
       </c>
@@ -7804,27 +8408,54 @@
       <c r="F22" s="5" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="5" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9739,7 +10370,7 @@
   <dimension ref="B2:J75"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
@@ -11997,15 +12628,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060CF4A208C699E48A9CAB1DE88D9955C" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9eb589bbb9ba3af1341624e6a0ce196">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a5fcea5b-d8c5-4ea2-9c68-e16cff4e4fdc" xmlns:ns3="4f835383-c8ab-4408-b923-549ff23016bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e76e43ba71ec876b5ee45d33cf470fb" ns2:_="" ns3:_="">
     <xsd:import namespace="a5fcea5b-d8c5-4ea2-9c68-e16cff4e4fdc"/>
@@ -12234,15 +12856,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7BF194-9CE8-44BF-AE79-5DB47C924373}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9DF2AD9-BA8E-4943-8F06-8F1CB1DBD300}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12259,4 +12882,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7BF194-9CE8-44BF-AE79-5DB47C924373}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated prod type Week5 Aug24
</commit_message>
<xml_diff>
--- a/0. Prod Inventory/Product Type_MY.xlsx
+++ b/0. Prod Inventory/Product Type_MY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nactuarialsolutions.sharepoint.com/sites/intern/Shared Documents/General/Product/web-scraper/0. Prod Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2893" documentId="13_ncr:1_{E59A9F57-7555-41DB-AD1E-6C065A761BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD6756BA-CFBE-4CDD-A94B-24851EFCDC68}"/>
+  <xr:revisionPtr revIDLastSave="3035" documentId="13_ncr:1_{E59A9F57-7555-41DB-AD1E-6C065A761BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AE6CD0A-A3B8-4C3D-87E7-55F1F6D23CF6}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="4" activeTab="4" xr2:uid="{70525E09-F0DC-4855-ADF9-7EA5A6A61783}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{70525E09-F0DC-4855-ADF9-7EA5A6A61783}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="9" r:id="rId1"/>
@@ -100,7 +100,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="3">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -115,20 +115,30 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="3">
     <bk>
       <rc t="1" v="0"/>
     </bk>
     <bk>
       <rc t="1" v="1"/>
     </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="711">
   <si>
     <t>Insurance Company</t>
   </si>
@@ -4175,6 +4185,181 @@
 &lt;70y: N/A
 &gt;=70y: Face Amount</t>
     </r>
+  </si>
+  <si>
+    <t>e-Takaful Hayat</t>
+  </si>
+  <si>
+    <t>SecurePro</t>
+  </si>
+  <si>
+    <t>Golden SeniorCare</t>
+  </si>
+  <si>
+    <t>17y-60y</t>
+  </si>
+  <si>
+    <t>Next Birthday</t>
+  </si>
+  <si>
+    <t>50y-70y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RM10k per unit 
+(Min 1 unit, Max 5 units)
+</t>
+  </si>
+  <si>
+    <t>Family Takaful with participant 
+account</t>
+  </si>
+  <si>
+    <t>From RM0.16/day</t>
+  </si>
+  <si>
+    <t>Up to 70y</t>
+  </si>
+  <si>
+    <t>3 plans available:
+RM50k/RM100k/RM200k</t>
+  </si>
+  <si>
+    <t>75% allocation</t>
+  </si>
+  <si>
+    <t>Additional 200% of SA</t>
+  </si>
+  <si>
+    <t>SA + RM1k compassionate benefit</t>
+  </si>
+  <si>
+    <t>RM1k compassionate benefit</t>
+  </si>
+  <si>
+    <t>From RM100/month</t>
+  </si>
+  <si>
+    <t>20 years or Up to 70y/80y/90y/100y</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Milestone Celebration Benefit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Can increase the 20% BSA (capped at RM100k) without underwriting when you celebrate life milestones, starting from the 3rd policy year onwards:
+a.    Graduation (tertiary and above or any equivalent);
+b.    Marriage;
+c.    Purchase of a new house; or
+d.    Birth of a newborn
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Loyalty bonus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> credited to your account automatically every 3 years from the 7th policy year onwards
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">No lapse guarantee </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Policy will remain in force and will not lapse for the first 6 policy years provided that no partial withdrawals are made and timely payments are made with no premium holidays.</t>
+    </r>
+  </si>
+  <si>
+    <t>Various CI riders, medical, accidental, lady care, WOP riders</t>
+  </si>
+  <si>
+    <t>Up to 100y</t>
+  </si>
+  <si>
+    <t>Limited pay, as short as 6 years</t>
+  </si>
+  <si>
+    <t>Y1-2: All premiums paid without interest
+Y3+: SA</t>
+  </si>
+  <si>
+    <t>Depends on Age at death:
+50y-64y: Additional 300% of SA
+65y-80y: Additional 150% of SA
+81y+: Additional 50% of SA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Emergency Care </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- For death occurring Y3+, 10% of the entitled death benefit will be payable as an emergency cash to the beneficiary supported by minimal documentation. The remaining sum will be payable upon receiving the complete documentation.</t>
+    </r>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>1m-35m: 100% of Guaranteed Surrender Value
+36m+: 20% of Guaranteed Surrender Value</t>
   </si>
 </sst>
 </file>
@@ -4258,7 +4443,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4310,6 +4495,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4445,7 +4636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4596,17 +4787,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="8" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4747,13 +4944,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>34018</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>415018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>4033</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>2536331</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5478,13 +5675,17 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
   <rv s="0">
     <v>0</v>
     <v>5</v>
   </rv>
   <rv s="0">
     <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -5503,6 +5704,7 @@
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
   <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
 </richValueRels>
 </file>
 
@@ -5837,25 +6039,25 @@
   </sheetPr>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="30" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="83.44140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="60.77734375" style="30" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="30"/>
+    <col min="1" max="1" width="6.796875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="28.53125" style="30" customWidth="1"/>
+    <col min="3" max="3" width="83.46484375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="60.796875" style="30" customWidth="1"/>
+    <col min="5" max="16384" width="8.86328125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="13.15" x14ac:dyDescent="0.45">
       <c r="A1" s="29" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="30">
         <v>1</v>
       </c>
@@ -5863,7 +6065,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -5871,7 +6073,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="30">
         <v>3</v>
       </c>
@@ -5879,7 +6081,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="30">
         <v>4</v>
       </c>
@@ -5887,7 +6089,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="30">
         <v>5</v>
       </c>
@@ -5895,12 +6097,12 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="13.15" x14ac:dyDescent="0.45">
       <c r="A26" s="29" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="13.15" x14ac:dyDescent="0.45">
       <c r="A27" s="31" t="s">
         <v>320</v>
       </c>
@@ -5914,7 +6116,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="32">
         <v>1</v>
       </c>
@@ -5928,7 +6130,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.45">
       <c r="A29" s="32">
         <f>A28+1</f>
         <v>2</v>
@@ -5943,7 +6145,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="63.75" x14ac:dyDescent="0.45">
       <c r="A30" s="32">
         <f t="shared" ref="A30:A49" si="0">A29+1</f>
         <v>3</v>
@@ -5958,7 +6160,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5973,7 +6175,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="89.25" x14ac:dyDescent="0.45">
       <c r="A32" s="32">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5988,7 +6190,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="250.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="229.5" x14ac:dyDescent="0.45">
       <c r="A33" s="32">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6003,7 +6205,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.45">
       <c r="A34" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6018,7 +6220,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6033,7 +6235,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6048,7 +6250,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="76.5" x14ac:dyDescent="0.45">
       <c r="A37" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6063,7 +6265,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="63.75" x14ac:dyDescent="0.45">
       <c r="A38" s="32">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6078,7 +6280,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="63.75" x14ac:dyDescent="0.45">
       <c r="A39" s="32">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6093,7 +6295,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="98" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="32">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6108,7 +6310,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="63.75" x14ac:dyDescent="0.45">
       <c r="A41" s="32">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -6123,7 +6325,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="89.25" x14ac:dyDescent="0.45">
       <c r="A42" s="32">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -6138,7 +6340,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="76.5" x14ac:dyDescent="0.45">
       <c r="A43" s="32">
         <f>A42+1</f>
         <v>16</v>
@@ -6153,7 +6355,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="76.5" x14ac:dyDescent="0.45">
       <c r="A44" s="32">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6168,7 +6370,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="63.75" x14ac:dyDescent="0.45">
       <c r="A45" s="32">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6183,7 +6385,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="63.75" x14ac:dyDescent="0.45">
       <c r="A46" s="32">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -6198,7 +6400,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="76.5" x14ac:dyDescent="0.45">
       <c r="A47" s="32">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6213,7 +6415,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="115.15" x14ac:dyDescent="0.45">
       <c r="A48" s="32">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -6228,7 +6430,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="102" x14ac:dyDescent="0.45">
       <c r="A49" s="32">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -6243,12 +6445,12 @@
         <v>354</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="13.15" x14ac:dyDescent="0.45">
       <c r="A54" s="29" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="13.15" x14ac:dyDescent="0.45">
       <c r="A55" s="31" t="s">
         <v>320</v>
       </c>
@@ -6259,7 +6461,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A56" s="32">
         <v>1</v>
       </c>
@@ -6270,7 +6472,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="32">
         <f>A56+1</f>
         <v>2</v>
@@ -6282,7 +6484,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="38.25" x14ac:dyDescent="0.45">
       <c r="A58" s="32">
         <f t="shared" ref="A58:A59" si="1">A57+1</f>
         <v>3</v>
@@ -6294,7 +6496,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="38.25" x14ac:dyDescent="0.45">
       <c r="A59" s="32">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -6306,7 +6508,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A60" s="32">
         <f>A59+1</f>
         <v>5</v>
@@ -6318,7 +6520,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A61" s="32">
         <f>A60+1</f>
         <v>6</v>
@@ -6339,28 +6541,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313B3ADD-1C7B-473A-99A9-A861CDD224A1}">
-  <dimension ref="B2:J23"/>
+  <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J2" sqref="J2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="81" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="19.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
+    <col min="2" max="2" width="19.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.46484375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52" style="1" customWidth="1"/>
     <col min="8" max="8" width="59.6640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="41.109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="10" width="41.1328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="29.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="56.53125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -6388,8 +6592,14 @@
       <c r="J2" s="3" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="54" t="s">
+        <v>685</v>
+      </c>
+      <c r="L2" s="54" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
@@ -6417,8 +6627,14 @@
       <c r="J3" s="2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="L3" s="58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -6446,8 +6662,14 @@
       <c r="J4" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
@@ -6475,8 +6697,14 @@
       <c r="J5" s="2" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K5" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -6504,8 +6732,14 @@
       <c r="J6" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
@@ -6533,8 +6767,14 @@
       <c r="J7" s="2" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="K7" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
@@ -6562,8 +6802,14 @@
       <c r="J8" s="2" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="K8" s="9" t="s">
+        <v>688</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="242.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
@@ -6591,27 +6837,33 @@
       <c r="J9" s="12" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K9" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="L9" s="9" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="57" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="57" t="s">
         <v>434</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="57" t="s">
         <v>579</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="57" t="s">
         <v>547</v>
       </c>
-      <c r="H10" s="54" t="s">
+      <c r="H10" s="57" t="s">
         <v>559</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -6620,27 +6872,39 @@
       <c r="J10" s="5" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="54"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="5" t="s">
         <v>577</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
@@ -6668,8 +6932,14 @@
       <c r="J12" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K12" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
@@ -6697,8 +6967,14 @@
       <c r="J13" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K13" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>97</v>
       </c>
@@ -6726,73 +7002,93 @@
       <c r="J14" s="17" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" ht="204" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+      <c r="K14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="H15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="I15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="J15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="K15" s="59" t="s">
+        <v>709</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="204" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="D16" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>548</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H16" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="J15" s="5" t="s">
+      <c r="I16" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+      <c r="K16" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D17" s="57" t="s">
         <v>248</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>588</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="120.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D17" s="54"/>
       <c r="E17" s="5" t="s">
         <v>171</v>
       </c>
@@ -6800,197 +7096,272 @@
         <v>171</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="K17" s="56" t="s">
+        <v>698</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="120.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="57"/>
+      <c r="E18" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
+      <c r="K18" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="E19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>504</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>589</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>534</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>64</v>
+        <v>563</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>589</v>
       </c>
       <c r="J19" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+      <c r="K20" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="E21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="5" t="s">
+      <c r="I21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="K21" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="57" x14ac:dyDescent="0.45">
+      <c r="B22" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="K22" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="270.75" x14ac:dyDescent="0.45">
+      <c r="B23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="E23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I22" s="5" t="s">
+      <c r="H23" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+      <c r="K23" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="G23" s="5" t="s">
+      <c r="E24" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J23" s="2" t="s">
+      <c r="I24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>594</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
@@ -7007,22 +7378,22 @@
   <dimension ref="B2:K31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="27.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.5546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="76.21875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
+    <col min="2" max="2" width="27.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.53125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="76.19921875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -7036,7 +7407,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
@@ -7050,7 +7421,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
@@ -7064,7 +7435,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -7078,7 +7449,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -7092,7 +7463,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -7106,7 +7477,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -7120,7 +7491,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -7137,7 +7508,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -7151,7 +7522,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -7165,7 +7536,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -7179,7 +7550,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
@@ -7193,7 +7564,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -7207,7 +7578,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="54" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -7221,7 +7592,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="213.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" ht="213.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
         <v>91</v>
       </c>
@@ -7235,7 +7606,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="13" t="s">
         <v>225</v>
       </c>
@@ -7243,7 +7614,7 @@
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
         <v>227</v>
       </c>
@@ -7257,7 +7628,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="92.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
         <v>228</v>
       </c>
@@ -7269,7 +7640,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
         <v>229</v>
       </c>
@@ -7281,7 +7652,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
         <v>230</v>
       </c>
@@ -7295,7 +7666,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
         <v>232</v>
       </c>
@@ -7309,7 +7680,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B23" s="4" t="s">
         <v>231</v>
       </c>
@@ -7323,7 +7694,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B24" s="13" t="s">
         <v>226</v>
       </c>
@@ -7331,7 +7702,7 @@
       <c r="D24" s="37"/>
       <c r="E24" s="37"/>
     </row>
-    <row r="25" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="4" t="s">
         <v>8</v>
       </c>
@@ -7345,7 +7716,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
         <v>9</v>
       </c>
@@ -7359,7 +7730,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" ht="57" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
@@ -7373,7 +7744,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
@@ -7387,7 +7758,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" ht="113.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="4" t="s">
         <v>19</v>
       </c>
@@ -7401,7 +7772,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="209.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" ht="209.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="4" t="s">
         <v>20</v>
       </c>
@@ -7415,7 +7786,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="358.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" ht="358.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="4" t="s">
         <v>14</v>
       </c>
@@ -7441,28 +7812,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48281F2A-1CEE-4910-884C-6FE42D909869}">
-  <dimension ref="B2:F32"/>
+  <dimension ref="B2:G32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="27.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
+    <col min="2" max="2" width="27.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.86328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="1" customWidth="1"/>
-    <col min="7" max="10" width="18.21875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="38.73046875" style="1" customWidth="1"/>
+    <col min="8" max="10" width="18.19921875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -7475,11 +7847,14 @@
       <c r="E2" s="9" t="s">
         <v>637</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="9" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="55" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
@@ -7495,8 +7870,11 @@
       <c r="F3" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
@@ -7512,8 +7890,11 @@
       <c r="F4" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -7529,8 +7910,11 @@
       <c r="F5" s="9" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -7546,8 +7930,11 @@
       <c r="F6" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -7563,8 +7950,11 @@
       <c r="F7" s="9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -7580,8 +7970,11 @@
       <c r="F8" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -7597,8 +7990,11 @@
       <c r="F9" s="9" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G9" s="9" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>390</v>
       </c>
@@ -7614,8 +8010,11 @@
       <c r="F10" s="5" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="9" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -7631,8 +8030,11 @@
       <c r="F11" s="5" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="9" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="47.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -7648,8 +8050,11 @@
       <c r="F12" s="5" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="47.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
@@ -7665,8 +8070,11 @@
       <c r="F13" s="5" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G13" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -7682,8 +8090,11 @@
       <c r="F14" s="5" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -7699,8 +8110,11 @@
       <c r="F15" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="156" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="156" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
         <v>394</v>
       </c>
@@ -7716,8 +8130,11 @@
       <c r="F16" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G16" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
         <v>91</v>
       </c>
@@ -7730,11 +8147,14 @@
       <c r="E17" s="28" t="s">
         <v>654</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="5" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="13" t="s">
         <v>225</v>
       </c>
@@ -7742,8 +8162,9 @@
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
-    </row>
-    <row r="19" spans="2:6" ht="263.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="37"/>
+    </row>
+    <row r="19" spans="2:7" ht="263.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
         <v>227</v>
       </c>
@@ -7759,8 +8180,11 @@
       <c r="F19" s="5" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" ht="143.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="143.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
         <v>228</v>
       </c>
@@ -7776,8 +8200,11 @@
       <c r="F20" s="5" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
         <v>229</v>
       </c>
@@ -7793,8 +8220,11 @@
       <c r="F21" s="5" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G21" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
         <v>230</v>
       </c>
@@ -7810,8 +8240,11 @@
       <c r="F22" s="39" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="4" t="s">
         <v>232</v>
       </c>
@@ -7827,8 +8260,11 @@
       <c r="F23" s="39" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G23" s="39" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
         <v>231</v>
       </c>
@@ -7844,8 +8280,11 @@
       <c r="F24" s="5" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" ht="231" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="231" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="4" t="s">
         <v>393</v>
       </c>
@@ -7861,8 +8300,11 @@
       <c r="F25" s="5" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B26" s="13" t="s">
         <v>226</v>
       </c>
@@ -7870,8 +8312,9 @@
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
       <c r="F26" s="37"/>
-    </row>
-    <row r="27" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="37"/>
+    </row>
+    <row r="27" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
@@ -7887,8 +8330,11 @@
       <c r="F27" s="5" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G27" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="57" x14ac:dyDescent="0.45">
       <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
@@ -7904,8 +8350,11 @@
       <c r="F28" s="5" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="G28" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B29" s="4" t="s">
         <v>221</v>
       </c>
@@ -7921,8 +8370,11 @@
       <c r="F29" s="5" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="115.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
@@ -7938,8 +8390,11 @@
       <c r="F30" s="9" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="G30" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="285" x14ac:dyDescent="0.45">
       <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
@@ -7955,8 +8410,11 @@
       <c r="F31" s="5" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" ht="372.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="372.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="4" t="s">
         <v>14</v>
       </c>
@@ -7971,6 +8429,9 @@
       </c>
       <c r="F32" s="9" t="s">
         <v>64</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>703</v>
       </c>
     </row>
   </sheetData>
@@ -7984,25 +8445,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8220FE-2D73-47FD-8C9B-E987A6F5AF90}">
   <dimension ref="B2:G24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="18.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
+    <col min="2" max="2" width="18.19921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.46484375" style="1" customWidth="1"/>
     <col min="5" max="6" width="30.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="64.21875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="64.19921875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -8022,7 +8483,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
@@ -8042,7 +8503,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
@@ -8062,7 +8523,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -8082,7 +8543,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -8102,7 +8563,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -8122,7 +8583,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -8142,7 +8603,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>176</v>
       </c>
@@ -8162,7 +8623,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -8178,11 +8639,11 @@
       <c r="F10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="2" t="e" vm="1">
+      <c r="G10" s="2" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -8202,7 +8663,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -8222,7 +8683,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
@@ -8242,7 +8703,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -8258,11 +8719,11 @@
       <c r="F14" s="12" t="s">
         <v>652</v>
       </c>
-      <c r="G14" s="12" t="e" vm="2">
+      <c r="G14" s="12" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -8282,7 +8743,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -8302,7 +8763,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="140.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
         <v>209</v>
       </c>
@@ -8322,7 +8783,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
@@ -8342,7 +8803,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="171" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
         <v>213</v>
       </c>
@@ -8362,7 +8823,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
@@ -8382,7 +8843,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
@@ -8392,7 +8853,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="2:7" ht="310.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="310.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
         <v>20</v>
       </c>
@@ -8412,27 +8873,27 @@
         <v>679</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="153.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="57" t="s">
+      <c r="C23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>64</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
@@ -8470,18 +8931,18 @@
       <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91" style="1" customWidth="1"/>
-    <col min="4" max="4" width="68.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="47.44140625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="53.88671875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="68.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="47.46484375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="53.86328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -8501,7 +8962,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
@@ -8521,7 +8982,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
@@ -8541,7 +9002,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -8561,7 +9022,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -8581,7 +9042,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -8601,7 +9062,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -8621,7 +9082,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -8641,7 +9102,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
@@ -8661,7 +9122,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
@@ -8681,7 +9142,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>472</v>
       </c>
@@ -8701,7 +9162,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
@@ -8721,7 +9182,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
@@ -8741,7 +9202,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
@@ -8761,7 +9222,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
@@ -8781,7 +9242,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
         <v>487</v>
       </c>
@@ -8801,7 +9262,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
         <v>474</v>
       </c>
@@ -8821,7 +9282,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
@@ -8841,7 +9302,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
@@ -8861,7 +9322,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
@@ -8881,7 +9342,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -8901,7 +9362,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="225.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="225.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="4" t="s">
         <v>260</v>
       </c>
@@ -8921,7 +9382,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="299.25" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
         <v>20</v>
       </c>
@@ -8941,7 +9402,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B25" s="4" t="s">
         <v>488</v>
       </c>
@@ -8951,7 +9412,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B26" s="48" t="s">
         <v>491</v>
       </c>
@@ -8971,7 +9432,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B27" s="22" t="s">
         <v>489</v>
       </c>
@@ -8991,7 +9452,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B28" s="47" t="s">
         <v>490</v>
       </c>
@@ -9011,7 +9472,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B29" s="22" t="s">
         <v>493</v>
       </c>
@@ -9031,7 +9492,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B30" s="22" t="s">
         <v>494</v>
       </c>
@@ -9051,7 +9512,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B31" s="22" t="s">
         <v>495</v>
       </c>
@@ -9071,7 +9532,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B32" s="22" t="s">
         <v>496</v>
       </c>
@@ -9091,7 +9552,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B33" s="22" t="s">
         <v>497</v>
       </c>
@@ -9111,7 +9572,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B34" s="22" t="s">
         <v>498</v>
       </c>
@@ -9131,7 +9592,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B35" s="20" t="s">
         <v>499</v>
       </c>
@@ -9151,7 +9612,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B36" s="20" t="s">
         <v>500</v>
       </c>
@@ -9171,7 +9632,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B37" s="4" t="s">
         <v>257</v>
       </c>
@@ -9181,7 +9642,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B38" s="21" t="s">
         <v>262</v>
       </c>
@@ -9199,7 +9660,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B39" s="22" t="s">
         <v>476</v>
       </c>
@@ -9215,7 +9676,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B40" s="47" t="s">
         <v>486</v>
       </c>
@@ -9231,7 +9692,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B41" s="22" t="s">
         <v>264</v>
       </c>
@@ -9249,7 +9710,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B42" s="22" t="s">
         <v>266</v>
       </c>
@@ -9267,7 +9728,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B43" s="22" t="s">
         <v>268</v>
       </c>
@@ -9285,7 +9746,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B44" s="22" t="s">
         <v>270</v>
       </c>
@@ -9303,7 +9764,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B45" s="22" t="s">
         <v>272</v>
       </c>
@@ -9323,7 +9784,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B46" s="22" t="s">
         <v>274</v>
       </c>
@@ -9341,7 +9802,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B47" s="20" t="s">
         <v>276</v>
       </c>
@@ -9359,7 +9820,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B48" s="20" t="s">
         <v>477</v>
       </c>
@@ -9375,7 +9836,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B49" s="20" t="s">
         <v>278</v>
       </c>
@@ -9393,7 +9854,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B50" s="19" t="s">
         <v>280</v>
       </c>
@@ -9411,7 +9872,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B51" s="19" t="s">
         <v>478</v>
       </c>
@@ -9427,7 +9888,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B52" s="19" t="s">
         <v>282</v>
       </c>
@@ -9445,7 +9906,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B53" s="19" t="s">
         <v>501</v>
       </c>
@@ -9457,7 +9918,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B54" s="19" t="s">
         <v>479</v>
       </c>
@@ -9473,7 +9934,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B55" s="19" t="s">
         <v>284</v>
       </c>
@@ -9491,7 +9952,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B56" s="19" t="s">
         <v>286</v>
       </c>
@@ -9509,7 +9970,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B57" s="19" t="s">
         <v>288</v>
       </c>
@@ -9527,7 +9988,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B58" s="19" t="s">
         <v>290</v>
       </c>
@@ -9545,7 +10006,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B59" s="19" t="s">
         <v>292</v>
       </c>
@@ -9563,7 +10024,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B60" s="19" t="s">
         <v>294</v>
       </c>
@@ -9581,7 +10042,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B61" s="19" t="s">
         <v>296</v>
       </c>
@@ -9599,7 +10060,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B62" s="6" t="s">
         <v>298</v>
       </c>
@@ -9617,7 +10078,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B63" s="22" t="s">
         <v>263</v>
       </c>
@@ -9635,7 +10096,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B64" s="22" t="s">
         <v>265</v>
       </c>
@@ -9653,7 +10114,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B65" s="22" t="s">
         <v>267</v>
       </c>
@@ -9671,7 +10132,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B66" s="22" t="s">
         <v>269</v>
       </c>
@@ -9689,7 +10150,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B67" s="22" t="s">
         <v>271</v>
       </c>
@@ -9707,7 +10168,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B68" s="22" t="s">
         <v>273</v>
       </c>
@@ -9725,7 +10186,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B69" s="22" t="s">
         <v>480</v>
       </c>
@@ -9741,7 +10202,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B70" s="22" t="s">
         <v>275</v>
       </c>
@@ -9759,7 +10220,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B71" s="22" t="s">
         <v>277</v>
       </c>
@@ -9777,7 +10238,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B72" s="6" t="s">
         <v>279</v>
       </c>
@@ -9795,7 +10256,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B73" s="6" t="s">
         <v>281</v>
       </c>
@@ -9813,7 +10274,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B74" s="6" t="s">
         <v>283</v>
       </c>
@@ -9831,7 +10292,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B75" s="6" t="s">
         <v>285</v>
       </c>
@@ -9849,7 +10310,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B76" s="6" t="s">
         <v>481</v>
       </c>
@@ -9865,7 +10326,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B77" s="6" t="s">
         <v>287</v>
       </c>
@@ -9883,7 +10344,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B78" s="6" t="s">
         <v>482</v>
       </c>
@@ -9899,7 +10360,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B79" s="6" t="s">
         <v>483</v>
       </c>
@@ -9915,7 +10376,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B80" s="6" t="s">
         <v>484</v>
       </c>
@@ -9931,7 +10392,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B81" s="6" t="s">
         <v>485</v>
       </c>
@@ -9947,7 +10408,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B82" s="6" t="s">
         <v>289</v>
       </c>
@@ -9965,7 +10426,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B83" s="6" t="s">
         <v>291</v>
       </c>
@@ -9983,7 +10444,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B84" s="6" t="s">
         <v>293</v>
       </c>
@@ -10001,7 +10462,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B85" s="6" t="s">
         <v>295</v>
       </c>
@@ -10019,7 +10480,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B86" s="6" t="s">
         <v>297</v>
       </c>
@@ -10037,7 +10498,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B87" s="6" t="s">
         <v>299</v>
       </c>
@@ -10055,7 +10516,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B88" s="4" t="s">
         <v>258</v>
       </c>
@@ -10065,7 +10526,7 @@
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B89" s="4" t="s">
         <v>24</v>
       </c>
@@ -10085,7 +10546,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="2:7" ht="173.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:7" ht="173.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B90" s="4" t="s">
         <v>26</v>
       </c>
@@ -10105,7 +10566,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B91" s="4" t="s">
         <v>39</v>
       </c>
@@ -10115,7 +10576,7 @@
       <c r="F91" s="26"/>
       <c r="G91" s="26"/>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B92" s="6" t="s">
         <v>30</v>
       </c>
@@ -10135,7 +10596,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B93" s="6" t="s">
         <v>31</v>
       </c>
@@ -10155,7 +10616,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B94" s="6" t="s">
         <v>32</v>
       </c>
@@ -10175,7 +10636,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B95" s="6" t="s">
         <v>33</v>
       </c>
@@ -10195,7 +10656,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B96" s="6" t="s">
         <v>34</v>
       </c>
@@ -10215,7 +10676,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B97" s="6" t="s">
         <v>35</v>
       </c>
@@ -10235,7 +10696,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B98" s="6" t="s">
         <v>36</v>
       </c>
@@ -10255,7 +10716,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B99" s="6" t="s">
         <v>37</v>
       </c>
@@ -10275,7 +10736,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B100" s="6" t="s">
         <v>38</v>
       </c>
@@ -10295,7 +10756,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B101" s="4" t="s">
         <v>40</v>
       </c>
@@ -10305,7 +10766,7 @@
       <c r="F101" s="27"/>
       <c r="G101" s="4"/>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B102" s="18" t="s">
         <v>41</v>
       </c>
@@ -10325,7 +10786,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B103" s="4" t="s">
         <v>42</v>
       </c>
@@ -10335,7 +10796,7 @@
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B104" s="8" t="s">
         <v>29</v>
       </c>
@@ -10376,19 +10837,19 @@
       <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="3" width="57.5546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="43.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="58.77734375" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="58.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="39.109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
+    <col min="2" max="3" width="57.53125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="43.86328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.796875" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="58.796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="39.1328125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -10417,7 +10878,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
@@ -10446,7 +10907,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
@@ -10475,7 +10936,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -10504,7 +10965,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -10533,7 +10994,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -10562,7 +11023,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -10587,7 +11048,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>176</v>
       </c>
@@ -10616,7 +11077,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
@@ -10645,7 +11106,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
@@ -10674,7 +11135,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
@@ -10703,7 +11164,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
@@ -10732,7 +11193,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -10761,7 +11222,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -10790,7 +11251,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -10819,7 +11280,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
@@ -10848,7 +11309,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
         <v>45</v>
       </c>
@@ -10877,7 +11338,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
         <v>180</v>
       </c>
@@ -10906,7 +11367,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
         <v>117</v>
       </c>
@@ -10935,7 +11396,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
@@ -10964,7 +11425,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="57" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
         <v>46</v>
       </c>
@@ -10993,7 +11454,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="13" t="s">
         <v>422</v>
       </c>
@@ -11006,7 +11467,7 @@
       <c r="I23" s="37"/>
       <c r="J23" s="37"/>
     </row>
-    <row r="24" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
         <v>394</v>
       </c>
@@ -11035,7 +11496,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="114" x14ac:dyDescent="0.45">
       <c r="B25" s="4" t="s">
         <v>91</v>
       </c>
@@ -11064,7 +11525,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
         <v>227</v>
       </c>
@@ -11093,7 +11554,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
         <v>228</v>
       </c>
@@ -11122,7 +11583,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="4" t="s">
         <v>229</v>
       </c>
@@ -11151,7 +11612,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" s="4" t="s">
         <v>230</v>
       </c>
@@ -11180,7 +11641,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B30" s="4" t="s">
         <v>232</v>
       </c>
@@ -11209,7 +11670,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B31" s="4" t="s">
         <v>231</v>
       </c>
@@ -11238,7 +11699,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B32" s="4" t="s">
         <v>393</v>
       </c>
@@ -11267,7 +11728,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B33" s="13" t="s">
         <v>119</v>
       </c>
@@ -11280,7 +11741,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B34" s="4" t="s">
         <v>47</v>
       </c>
@@ -11309,7 +11770,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B35" s="4" t="s">
         <v>93</v>
       </c>
@@ -11338,7 +11799,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B36" s="4" t="s">
         <v>96</v>
       </c>
@@ -11367,7 +11828,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" s="4" t="s">
         <v>94</v>
       </c>
@@ -11396,7 +11857,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="4" t="s">
         <v>95</v>
       </c>
@@ -11425,7 +11886,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" s="4" t="s">
         <v>105</v>
       </c>
@@ -11454,7 +11915,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B40" s="4" t="s">
         <v>106</v>
       </c>
@@ -11483,7 +11944,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B41" s="4" t="s">
         <v>107</v>
       </c>
@@ -11512,7 +11973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B42" s="4" t="s">
         <v>463</v>
       </c>
@@ -11541,7 +12002,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" s="4" t="s">
         <v>462</v>
       </c>
@@ -11570,7 +12031,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B44" s="4" t="s">
         <v>403</v>
       </c>
@@ -11599,7 +12060,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B45" s="13" t="s">
         <v>120</v>
       </c>
@@ -11612,7 +12073,7 @@
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
     </row>
-    <row r="46" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B46" s="4" t="s">
         <v>108</v>
       </c>
@@ -11641,7 +12102,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="47" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B47" s="4" t="s">
         <v>109</v>
       </c>
@@ -11670,7 +12131,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B48" s="4" t="s">
         <v>185</v>
       </c>
@@ -11699,7 +12160,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B49" s="13" t="s">
         <v>121</v>
       </c>
@@ -11712,7 +12173,7 @@
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B50" s="4" t="s">
         <v>187</v>
       </c>
@@ -11741,7 +12202,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B51" s="4" t="s">
         <v>188</v>
       </c>
@@ -11770,7 +12231,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B52" s="4" t="s">
         <v>405</v>
       </c>
@@ -11799,7 +12260,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:10" ht="57" x14ac:dyDescent="0.45">
       <c r="B53" s="4" t="s">
         <v>459</v>
       </c>
@@ -11828,7 +12289,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B54" s="4" t="s">
         <v>458</v>
       </c>
@@ -11857,7 +12318,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B55" s="13" t="s">
         <v>122</v>
       </c>
@@ -11870,7 +12331,7 @@
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B56" s="4" t="s">
         <v>110</v>
       </c>
@@ -11899,7 +12360,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B57" s="4" t="s">
         <v>111</v>
       </c>
@@ -11928,7 +12389,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B58" s="4" t="s">
         <v>460</v>
       </c>
@@ -11957,7 +12418,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="2:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:10" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B59" s="4" t="s">
         <v>144</v>
       </c>
@@ -11986,7 +12447,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:10" ht="57" x14ac:dyDescent="0.45">
       <c r="B60" s="4" t="s">
         <v>192</v>
       </c>
@@ -12015,7 +12476,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B61" s="4" t="s">
         <v>112</v>
       </c>
@@ -12044,7 +12505,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="62" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B62" s="4" t="s">
         <v>113</v>
       </c>
@@ -12073,7 +12534,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B63" s="13" t="s">
         <v>123</v>
       </c>
@@ -12086,7 +12547,7 @@
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
     </row>
-    <row r="64" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B64" s="4" t="s">
         <v>146</v>
       </c>
@@ -12115,7 +12576,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:10" ht="57" x14ac:dyDescent="0.45">
       <c r="B65" s="4" t="s">
         <v>418</v>
       </c>
@@ -12144,7 +12605,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:10" ht="57" x14ac:dyDescent="0.45">
       <c r="B66" s="4" t="s">
         <v>414</v>
       </c>
@@ -12173,7 +12634,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B67" s="4" t="s">
         <v>195</v>
       </c>
@@ -12202,7 +12663,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="2:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:10" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B68" s="4" t="s">
         <v>114</v>
       </c>
@@ -12231,7 +12692,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="2:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:10" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B69" s="4" t="s">
         <v>115</v>
       </c>
@@ -12260,7 +12721,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B70" s="4" t="s">
         <v>465</v>
       </c>
@@ -12289,7 +12750,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B71" s="4" t="s">
         <v>49</v>
       </c>
@@ -12318,7 +12779,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B72" s="4" t="s">
         <v>48</v>
       </c>
@@ -12347,7 +12808,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="2:10" ht="288" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:10" ht="285" x14ac:dyDescent="0.45">
       <c r="B73" s="4" t="s">
         <v>197</v>
       </c>
@@ -12376,7 +12837,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="2:10" ht="360" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:10" ht="342" x14ac:dyDescent="0.45">
       <c r="B74" s="4" t="s">
         <v>20</v>
       </c>
@@ -12405,7 +12866,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="75" spans="2:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:10" ht="199.5" x14ac:dyDescent="0.45">
       <c r="B75" s="4" t="s">
         <v>14</v>
       </c>
@@ -12453,15 +12914,15 @@
       <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="59.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
+    <col min="2" max="2" width="59.796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="91" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -12469,7 +12930,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -12477,7 +12938,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>152</v>
       </c>
@@ -12485,7 +12946,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
@@ -12493,7 +12954,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -12501,7 +12962,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="2:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
@@ -12509,7 +12970,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
@@ -12517,7 +12978,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
@@ -12525,7 +12986,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -12533,7 +12994,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -12541,7 +13002,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -12549,7 +13010,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
@@ -12557,7 +13018,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -12565,7 +13026,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -12573,7 +13034,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
@@ -12581,7 +13042,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
@@ -12589,7 +13050,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
@@ -12597,7 +13058,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="173.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" ht="173.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
@@ -12605,7 +13066,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="244.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="244.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
         <v>27</v>
       </c>
@@ -12613,7 +13074,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" ht="53.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
         <v>28</v>
       </c>

</xml_diff>